<commit_message>
Committing the AVS scripts
</commit_message>
<xml_diff>
--- a/TestData/UserManagementTestData.xlsx
+++ b/TestData/UserManagementTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stored-Code\TestAutomation\Development\Root\Source\VRT\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruchika.Behura\git\AVS\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F55239-74B3-4E80-A512-668C5E6D1360}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06355CA4-A525-4205-A379-5DD708FFDDEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="9" activeTab="14" xr2:uid="{FFF56094-AA49-43C9-8779-4520FC744D16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="15" xr2:uid="{FFF56094-AA49-43C9-8779-4520FC744D16}"/>
   </bookViews>
   <sheets>
     <sheet name="tcADMN124" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,8 @@
     <sheet name="tcADMN159" sheetId="17" r:id="rId13"/>
     <sheet name="tcADMN160" sheetId="18" r:id="rId14"/>
     <sheet name="tcADMN188a" sheetId="19" r:id="rId15"/>
+    <sheet name="UAM030A" sheetId="20" r:id="rId16"/>
+    <sheet name="Sheet2" sheetId="21" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -342,6 +344,36 @@
   </si>
   <si>
     <t>User Id cannot be blank. Please provide valid User Id.</t>
+  </si>
+  <si>
+    <t>AName</t>
+  </si>
+  <si>
+    <t>AID</t>
+  </si>
+  <si>
+    <t>AType</t>
+  </si>
+  <si>
+    <t>Amanufacturer</t>
+  </si>
+  <si>
+    <t>ALocation</t>
+  </si>
+  <si>
+    <t>ADMIN074</t>
+  </si>
+  <si>
+    <t>074</t>
+  </si>
+  <si>
+    <t>HeatBath</t>
+  </si>
+  <si>
+    <t>Htc</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
   </si>
 </sst>
 </file>
@@ -457,7 +489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -531,6 +563,8 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1715,7 +1749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9AC851-843F-4311-966F-386BB924662B}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1770,6 +1804,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA06B64-2AE1-4FB1-847F-9AD0CD952A24}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30433007-76DC-4F9B-8891-9882029BBF5B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>